<commit_message>
Add kibot:JLC:pricing from existing columns
</commit_message>
<xml_diff>
--- a/board/output/OBSPro-kicost.xlsx
+++ b/board/output/OBSPro-kicost.xlsx
@@ -271,9 +271,585 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $1.03      $1.03
-    10   $0.97      $9.65
+    10   $0.87      $8.65
    100   $0.57     $57.24
   1000   $0.61    $606.50</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.06      $0.06
+    10   $0.01      $0.06
+   100   $0.00      $0.31
+  1000   $0.00      $2.90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.06      $0.06
+    10   $0.01      $0.06
+   100   $0.00      $0.28
+  1000   $0.00      $2.70</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.04      $0.04
+    10   $0.00      $0.04
+   100   $0.00      $0.21
+  1000   $0.00      $1.40</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.06      $0.06
+    10   $0.01      $0.06
+   100   $0.00      $0.31
+  1000   $0.00      $2.90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.11      $0.11
+    10   $0.01      $0.11
+   100   $0.01      $0.53
+  1000   $0.00      $3.60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.17      $0.17
+    10   $0.13      $1.31
+   100   $0.10      $9.72
+  1000   $0.09     $90.20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.16      $0.16
+    10   $0.13      $1.31
+   100   $0.10      $9.98
+  1000   $0.09     $93.30</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.11      $0.11
+    10   $0.04      $0.44
+   100   $0.02      $1.79
+  1000   $0.01     $14.20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $1.54      $1.54
+    10   $1.30     $12.98
+   100   $1.17    $116.71
+  1000   $1.02  $1,017.90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $1.54      $1.54
+    10   $1.30     $12.98
+   100   $1.17    $116.71
+  1000   $1.02  $1,017.90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.18      $0.18
+    10   $0.02      $0.18
+   100   $0.01      $1.37
+  1000   $0.01     $10.70</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.22      $0.22
+    10   $0.02      $0.22
+   100   $0.01      $1.44
+  1000   $0.01      $9.80</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $2.10      $2.10
+    10   $1.85     $18.52
+   100   $1.52    $151.55
+  1000   $1.41  $1,410.50</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $2.45      $2.45
+    10   $2.45     $24.48
+   100   $2.36    $235.71
+  1000   $2.36  $2,357.10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.72      $0.72
+    10   $0.71      $7.08
+   100   $0.71     $70.84
+  1000   $0.71    $708.40</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1  $21.00     $21.00
+    10  $15.73    $157.30
+   100  $10.32  $1,032.00
+  1000  $10.32 $10,320.00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.12      $0.12
+    10   $0.10      $0.97
+   100   $0.07      $7.28
+  1000   $0.07     $69.60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not stocked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Qty/Price Breaks (USD):
+  Qty  -  Unit$  -  Ext$
+================
+     1   $0.16      $0.16
+    10   $0.08      $0.82
+   100   $0.06      $5.76
+  1000   $0.05     $46.40</t>
         </r>
       </text>
     </comment>
@@ -321,7 +897,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="162">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -788,7 +1364,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Thu 24 Nov 2022 11:31:06 AM CET</t>
+    <t>Thu 24 Nov 2022 03:08:04 PM CET</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -803,7 +1379,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-11-24 11:31:08</t>
+    <t>2022-11-24 15:08:06</t>
   </si>
   <si>
     <t>KiCost® v1.1.12</t>
@@ -1356,7 +1932,7 @@
       </c>
       <c r="H2" s="4">
         <f>TotalCost/BoardQty</f>
-        <v>0.5544</v>
+        <v>20.0326</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1371,15 +1947,15 @@
       </c>
       <c r="H3" s="5">
         <f>SUM(H7:H52)</f>
-        <v>55.4383</v>
+        <v>2003.2639</v>
       </c>
       <c r="M3" s="5">
         <f>SUM(M7:M52)</f>
-        <v>55.4383</v>
+        <v>2003.2639</v>
       </c>
       <c r="N3" s="6" t="str">
         <f>(COUNTA(M7:M52)&amp;" of "&amp;ROWS(M7:M52)&amp;" parts found")</f>
-        <v>1 of 46 parts found</v>
+        <v>19 of 46 parts found</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1484,7 +2060,7 @@
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="11">
-        <f>IFERROR(IF(OR(J7&gt;=L7,F7&gt;=L7),EUR_USD*LOOKUP(IF(J7="",F7,J7),{0,1,10,100,1000},{0.0,1.0297,0.9651,0.5724,0.6065}),"MOQ="&amp;L7),"")</f>
+        <f>IFERROR(IF(OR(J7&gt;=L7,F7&gt;=L7),EUR_USD*LOOKUP(IF(J7="",F7,J7),{0,1,10,100,1000},{0.0,1.0297,0.8651,0.5724,0.6065}),"MOQ="&amp;L7),"")</f>
         <v>0.5543825665859564</v>
       </c>
       <c r="L7" s="10">
@@ -1540,11 +2116,29 @@
       </c>
       <c r="G9" s="11">
         <f>IF(MIN(K9)&lt;&gt;0,MIN(K9),"")</f>
-        <v/>
+        <v>0.003002421307506053</v>
       </c>
       <c r="H9" s="12">
         <f>IF(AND(ISNUMBER(F9),ISNUMBER(G9)),F9*G9,"")</f>
-        <v/>
+        <v>0.6005</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11">
+        <f>IFERROR(IF(OR(J9&gt;=L9,F9&gt;=L9),EUR_USD*LOOKUP(IF(J9="",F9,J9),{0,1,10,100,1000},{0.0,0.062,0.0062,0.0031,0.0029}),"MOQ="&amp;L9),"")</f>
+        <v>0.003002421307506053</v>
+      </c>
+      <c r="L9" s="10">
+        <v>1</v>
+      </c>
+      <c r="M9" s="12">
+        <f>IFERROR(IF(J9="",F9,J9)*K9,"")</f>
+        <v>0.6005</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1595,11 +2189,29 @@
       </c>
       <c r="G11" s="11">
         <f>IF(MIN(K11)&lt;&gt;0,MIN(K11),"")</f>
-        <v/>
+        <v>0.002711864406779661</v>
       </c>
       <c r="H11" s="12">
         <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
-        <v/>
+        <v>0.5424</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="11">
+        <f>IFERROR(IF(OR(J11&gt;=L11,F11&gt;=L11),EUR_USD*LOOKUP(IF(J11="",F11,J11),{0,1,10,100,1000},{0.0,0.056,0.0056,0.0028,0.0027}),"MOQ="&amp;L11),"")</f>
+        <v>0.002711864406779661</v>
+      </c>
+      <c r="L11" s="10">
+        <v>1</v>
+      </c>
+      <c r="M11" s="12">
+        <f>IFERROR(IF(J11="",F11,J11)*K11,"")</f>
+        <v>0.5424</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1621,11 +2233,29 @@
       </c>
       <c r="G12" s="11">
         <f>IF(MIN(K12)&lt;&gt;0,MIN(K12),"")</f>
-        <v/>
+        <v>0.002033898305084746</v>
       </c>
       <c r="H12" s="12">
         <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
-        <v/>
+        <v>1.4237</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11">
+        <f>IFERROR(IF(OR(J12&gt;=L12,F12&gt;=L12),EUR_USD*LOOKUP(IF(J12="",F12,J12),{0,1,10,100,1000},{0.0,0.042,0.0042,0.0021,0.0014}),"MOQ="&amp;L12),"")</f>
+        <v>0.002033898305084746</v>
+      </c>
+      <c r="L12" s="10">
+        <v>1</v>
+      </c>
+      <c r="M12" s="12">
+        <f>IFERROR(IF(J12="",F12,J12)*K12,"")</f>
+        <v>1.4237</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1647,11 +2277,29 @@
       </c>
       <c r="G13" s="11">
         <f>IF(MIN(K13)&lt;&gt;0,MIN(K13),"")</f>
-        <v/>
+        <v>0.003002421307506053</v>
       </c>
       <c r="H13" s="12">
         <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
-        <v/>
+        <v>0.3002</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11">
+        <f>IFERROR(IF(OR(J13&gt;=L13,F13&gt;=L13),EUR_USD*LOOKUP(IF(J13="",F13,J13),{0,1,10,100,1000},{0.0,0.062,0.0062,0.0031,0.0029}),"MOQ="&amp;L13),"")</f>
+        <v>0.003002421307506053</v>
+      </c>
+      <c r="L13" s="10">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12">
+        <f>IFERROR(IF(J13="",F13,J13)*K13,"")</f>
+        <v>0.3002</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1714,7 +2362,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:14">
       <c r="A17" s="10" t="s">
         <v>38</v>
       </c>
@@ -1736,14 +2384,32 @@
       </c>
       <c r="G17" s="11">
         <f>IF(MIN(K17)&lt;&gt;0,MIN(K17),"")</f>
-        <v/>
+        <v>0.00513317191283293</v>
       </c>
       <c r="H17" s="12">
         <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>1.0266</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11">
+        <f>IFERROR(IF(OR(J17&gt;=L17,F17&gt;=L17),EUR_USD*LOOKUP(IF(J17="",F17,J17),{0,1,10,100,1000},{0.0,0.106,0.0106,0.0053,0.0036}),"MOQ="&amp;L17),"")</f>
+        <v>0.00513317191283293</v>
+      </c>
+      <c r="L17" s="10">
+        <v>1</v>
+      </c>
+      <c r="M17" s="12">
+        <f>IFERROR(IF(J17="",F17,J17)*K17,"")</f>
+        <v>1.0266</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="10" t="s">
         <v>43</v>
       </c>
@@ -1763,7 +2429,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:14">
       <c r="A19" s="10" t="s">
         <v>45</v>
       </c>
@@ -1782,14 +2448,32 @@
       </c>
       <c r="G19" s="11">
         <f>IF(MIN(K19)&lt;&gt;0,MIN(K19),"")</f>
-        <v/>
+        <v>0.09414043583535109</v>
       </c>
       <c r="H19" s="12">
         <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>9.414</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11">
+        <f>IFERROR(IF(OR(J19&gt;=L19,F19&gt;=L19),EUR_USD*LOOKUP(IF(J19="",F19,J19),{0,1,10,100,1000},{0.0,0.1675,0.1309,0.0972,0.0902}),"MOQ="&amp;L19),"")</f>
+        <v>0.09414043583535109</v>
+      </c>
+      <c r="L19" s="10">
+        <v>1</v>
+      </c>
+      <c r="M19" s="12">
+        <f>IFERROR(IF(J19="",F19,J19)*K19,"")</f>
+        <v>9.414</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="10" t="s">
         <v>49</v>
       </c>
@@ -1811,14 +2495,32 @@
       </c>
       <c r="G20" s="11">
         <f>IF(MIN(K20)&lt;&gt;0,MIN(K20),"")</f>
-        <v/>
+        <v>0.09665859564164649</v>
       </c>
       <c r="H20" s="12">
         <f>IF(AND(ISNUMBER(F20),ISNUMBER(G20)),F20*G20,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>9.6659</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11">
+        <f>IFERROR(IF(OR(J20&gt;=L20,F20&gt;=L20),EUR_USD*LOOKUP(IF(J20="",F20,J20),{0,1,10,100,1000},{0.0,0.1646,0.131,0.0998,0.0933}),"MOQ="&amp;L20),"")</f>
+        <v>0.09665859564164649</v>
+      </c>
+      <c r="L20" s="10">
+        <v>1</v>
+      </c>
+      <c r="M20" s="12">
+        <f>IFERROR(IF(J20="",F20,J20)*K20,"")</f>
+        <v>9.6659</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
@@ -1838,7 +2540,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:14">
       <c r="A22" s="10" t="s">
         <v>54</v>
       </c>
@@ -1857,14 +2559,32 @@
       </c>
       <c r="G22" s="11">
         <f>IF(MIN(K22)&lt;&gt;0,MIN(K22),"")</f>
-        <v/>
+        <v>0.017336561743341403</v>
       </c>
       <c r="H22" s="12">
         <f>IF(AND(ISNUMBER(F22),ISNUMBER(G22)),F22*G22,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>1.7337</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11">
+        <f>IFERROR(IF(OR(J22&gt;=L22,F22&gt;=L22),EUR_USD*LOOKUP(IF(J22="",F22,J22),{0,1,10,100,1000},{0.0,0.1105,0.0442,0.0179,0.0142}),"MOQ="&amp;L22),"")</f>
+        <v>0.017336561743341403</v>
+      </c>
+      <c r="L22" s="10">
+        <v>1</v>
+      </c>
+      <c r="M22" s="12">
+        <f>IFERROR(IF(J22="",F22,J22)*K22,"")</f>
+        <v>1.7337</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="10" t="s">
         <v>58</v>
       </c>
@@ -1893,7 +2613,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:14">
       <c r="A24" s="10" t="s">
         <v>62</v>
       </c>
@@ -1912,14 +2632,32 @@
       </c>
       <c r="G24" s="11">
         <f>IF(MIN(K24)&lt;&gt;0,MIN(K24),"")</f>
-        <v/>
+        <v>1.130363196125908</v>
       </c>
       <c r="H24" s="12">
         <f>IF(AND(ISNUMBER(F24),ISNUMBER(G24)),F24*G24,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>226.0726</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11">
+        <f>IFERROR(IF(OR(J24&gt;=L24,F24&gt;=L24),EUR_USD*LOOKUP(IF(J24="",F24,J24),{0,1,10,100,1000},{0.0,1.5383,1.2985,1.1671,1.0179}),"MOQ="&amp;L24),"")</f>
+        <v>1.130363196125908</v>
+      </c>
+      <c r="L24" s="10">
+        <v>1</v>
+      </c>
+      <c r="M24" s="12">
+        <f>IFERROR(IF(J24="",F24,J24)*K24,"")</f>
+        <v>226.0726</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="10" t="s">
         <v>66</v>
       </c>
@@ -1938,14 +2676,32 @@
       </c>
       <c r="G25" s="11">
         <f>IF(MIN(K25)&lt;&gt;0,MIN(K25),"")</f>
-        <v/>
+        <v>1.130363196125908</v>
       </c>
       <c r="H25" s="12">
         <f>IF(AND(ISNUMBER(F25),ISNUMBER(G25)),F25*G25,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>226.0726</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="11">
+        <f>IFERROR(IF(OR(J25&gt;=L25,F25&gt;=L25),EUR_USD*LOOKUP(IF(J25="",F25,J25),{0,1,10,100,1000},{0.0,1.5383,1.2985,1.1671,1.0179}),"MOQ="&amp;L25),"")</f>
+        <v>1.130363196125908</v>
+      </c>
+      <c r="L25" s="10">
+        <v>1</v>
+      </c>
+      <c r="M25" s="12">
+        <f>IFERROR(IF(J25="",F25,J25)*K25,"")</f>
+        <v>226.0726</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="10" t="s">
         <v>68</v>
       </c>
@@ -1964,14 +2720,32 @@
       </c>
       <c r="G26" s="11">
         <f>IF(MIN(K26)&lt;&gt;0,MIN(K26),"")</f>
-        <v/>
+        <v>0.013268765133171913</v>
       </c>
       <c r="H26" s="12">
         <f>IF(AND(ISNUMBER(F26),ISNUMBER(G26)),F26*G26,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1">
+        <v>5.3075</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="11">
+        <f>IFERROR(IF(OR(J26&gt;=L26,F26&gt;=L26),EUR_USD*LOOKUP(IF(J26="",F26,J26),{0,1,10,100,1000},{0.0,0.176,0.0176,0.0137,0.0107}),"MOQ="&amp;L26),"")</f>
+        <v>0.013268765133171913</v>
+      </c>
+      <c r="L26" s="10">
+        <v>1</v>
+      </c>
+      <c r="M26" s="12">
+        <f>IFERROR(IF(J26="",F26,J26)*K26,"")</f>
+        <v>5.3075</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>71</v>
       </c>
@@ -1990,14 +2764,32 @@
       </c>
       <c r="G27" s="11">
         <f>IF(MIN(K27)&lt;&gt;0,MIN(K27),"")</f>
-        <v/>
+        <v>0.013946731234866828</v>
       </c>
       <c r="H27" s="12">
         <f>IF(AND(ISNUMBER(F27),ISNUMBER(G27)),F27*G27,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>2.7893</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="11">
+        <f>IFERROR(IF(OR(J27&gt;=L27,F27&gt;=L27),EUR_USD*LOOKUP(IF(J27="",F27,J27),{0,1,10,100,1000},{0.0,0.216,0.0216,0.0144,0.0098}),"MOQ="&amp;L27),"")</f>
+        <v>0.013946731234866828</v>
+      </c>
+      <c r="L27" s="10">
+        <v>1</v>
+      </c>
+      <c r="M27" s="12">
+        <f>IFERROR(IF(J27="",F27,J27)*K27,"")</f>
+        <v>2.7893</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="10" t="s">
         <v>75</v>
       </c>
@@ -2017,7 +2809,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:14">
       <c r="A29" s="10" t="s">
         <v>77</v>
       </c>
@@ -2046,7 +2838,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:14">
       <c r="A30" s="10" t="s">
         <v>82</v>
       </c>
@@ -2075,7 +2867,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:14">
       <c r="A31" s="10" t="s">
         <v>85</v>
       </c>
@@ -2104,7 +2896,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:14">
       <c r="A32" s="10" t="s">
         <v>88</v>
       </c>
@@ -2124,7 +2916,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:14">
       <c r="A33" s="10" t="s">
         <v>90</v>
       </c>
@@ -2144,7 +2936,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:14">
       <c r="A34" s="10" t="s">
         <v>92</v>
       </c>
@@ -2164,7 +2956,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:14">
       <c r="A35" s="10" t="s">
         <v>94</v>
       </c>
@@ -2184,7 +2976,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:14">
       <c r="A36" s="10" t="s">
         <v>96</v>
       </c>
@@ -2204,7 +2996,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:14">
       <c r="A37" s="10" t="s">
         <v>97</v>
       </c>
@@ -2224,7 +3016,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:14">
       <c r="A38" s="10" t="s">
         <v>99</v>
       </c>
@@ -2244,7 +3036,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:14">
       <c r="A39" s="10" t="s">
         <v>101</v>
       </c>
@@ -2264,7 +3056,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:14">
       <c r="A40" s="10" t="s">
         <v>103</v>
       </c>
@@ -2284,7 +3076,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:14">
       <c r="A41" s="10" t="s">
         <v>105</v>
       </c>
@@ -2304,7 +3096,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:14">
       <c r="A42" s="10" t="s">
         <v>107</v>
       </c>
@@ -2324,7 +3116,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:14">
       <c r="A43" s="10" t="s">
         <v>109</v>
       </c>
@@ -2344,7 +3136,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:14">
       <c r="A44" s="10" t="s">
         <v>111</v>
       </c>
@@ -2364,7 +3156,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:14">
       <c r="A45" s="10" t="s">
         <v>113</v>
       </c>
@@ -2384,7 +3176,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30" customHeight="1">
+    <row r="46" spans="1:14" ht="30" customHeight="1">
       <c r="A46" s="10" t="s">
         <v>115</v>
       </c>
@@ -2406,14 +3198,32 @@
       </c>
       <c r="G46" s="11">
         <f>IF(MIN(K46)&lt;&gt;0,MIN(K46),"")</f>
-        <v/>
+        <v>1.4677966101694917</v>
       </c>
       <c r="H46" s="12">
         <f>IF(AND(ISNUMBER(F46),ISNUMBER(G46)),F46*G46,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>146.7797</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J46" s="10"/>
+      <c r="K46" s="11">
+        <f>IFERROR(IF(OR(J46&gt;=L46,F46&gt;=L46),EUR_USD*LOOKUP(IF(J46="",F46,J46),{0,1,10,100,1000},{0.0,2.1016,1.8524,1.5155,1.4105}),"MOQ="&amp;L46),"")</f>
+        <v>1.4677966101694917</v>
+      </c>
+      <c r="L46" s="10">
+        <v>1</v>
+      </c>
+      <c r="M46" s="12">
+        <f>IFERROR(IF(J46="",F46,J46)*K46,"")</f>
+        <v>146.7797</v>
+      </c>
+      <c r="N46" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="10" t="s">
         <v>120</v>
       </c>
@@ -2435,14 +3245,32 @@
       </c>
       <c r="G47" s="11">
         <f>IF(MIN(K47)&lt;&gt;0,MIN(K47),"")</f>
-        <v/>
+        <v>2.282905569007264</v>
       </c>
       <c r="H47" s="12">
         <f>IF(AND(ISNUMBER(F47),ISNUMBER(G47)),F47*G47,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>228.2906</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="10"/>
+      <c r="K47" s="11">
+        <f>IFERROR(IF(OR(J47&gt;=L47,F47&gt;=L47),EUR_USD*LOOKUP(IF(J47="",F47,J47),{0,1,10,100,1000},{0.0,2.448,2.448,2.3571,2.3571}),"MOQ="&amp;L47),"")</f>
+        <v>2.282905569007264</v>
+      </c>
+      <c r="L47" s="10">
+        <v>1</v>
+      </c>
+      <c r="M47" s="12">
+        <f>IFERROR(IF(J47="",F47,J47)*K47,"")</f>
+        <v>228.2906</v>
+      </c>
+      <c r="N47" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="10" t="s">
         <v>123</v>
       </c>
@@ -2464,14 +3292,32 @@
       </c>
       <c r="G48" s="11">
         <f>IF(MIN(K48)&lt;&gt;0,MIN(K48),"")</f>
-        <v/>
+        <v>0.6861016949152543</v>
       </c>
       <c r="H48" s="12">
         <f>IF(AND(ISNUMBER(F48),ISNUMBER(G48)),F48*G48,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
+        <v>68.6102</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J48" s="10"/>
+      <c r="K48" s="11">
+        <f>IFERROR(IF(OR(J48&gt;=L48,F48&gt;=L48),EUR_USD*LOOKUP(IF(J48="",F48,J48),{0,1,10,100,1000},{0.0,0.7209,0.7084,0.7084,0.7084}),"MOQ="&amp;L48),"")</f>
+        <v>0.6861016949152543</v>
+      </c>
+      <c r="L48" s="10">
+        <v>1</v>
+      </c>
+      <c r="M48" s="12">
+        <f>IFERROR(IF(J48="",F48,J48)*K48,"")</f>
+        <v>68.6102</v>
+      </c>
+      <c r="N48" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="10" t="s">
         <v>128</v>
       </c>
@@ -2493,14 +3339,32 @@
       </c>
       <c r="G49" s="11">
         <f>IF(MIN(K49)&lt;&gt;0,MIN(K49),"")</f>
-        <v/>
+        <v>9.995157384987893</v>
       </c>
       <c r="H49" s="12">
         <f>IF(AND(ISNUMBER(F49),ISNUMBER(G49)),F49*G49,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
+        <v>999.5157</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J49" s="10"/>
+      <c r="K49" s="11">
+        <f>IFERROR(IF(OR(J49&gt;=L49,F49&gt;=L49),EUR_USD*LOOKUP(IF(J49="",F49,J49),{0,1,10,100,1000},{0.0,21.0,15.73,10.32,10.32}),"MOQ="&amp;L49),"")</f>
+        <v>9.995157384987893</v>
+      </c>
+      <c r="L49" s="10">
+        <v>1</v>
+      </c>
+      <c r="M49" s="12">
+        <f>IFERROR(IF(J49="",F49,J49)*K49,"")</f>
+        <v>999.5157</v>
+      </c>
+      <c r="N49" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="10" t="s">
         <v>133</v>
       </c>
@@ -2519,14 +3383,32 @@
       </c>
       <c r="G50" s="11">
         <f>IF(MIN(K50)&lt;&gt;0,MIN(K50),"")</f>
-        <v/>
+        <v>0.07050847457627119</v>
       </c>
       <c r="H50" s="12">
         <f>IF(AND(ISNUMBER(F50),ISNUMBER(G50)),F50*G50,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
+        <v>14.1017</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J50" s="10"/>
+      <c r="K50" s="11">
+        <f>IFERROR(IF(OR(J50&gt;=L50,F50&gt;=L50),EUR_USD*LOOKUP(IF(J50="",F50,J50),{0,1,10,100,1000},{0.0,0.1235,0.0971,0.0728,0.0696}),"MOQ="&amp;L50),"")</f>
+        <v>0.07050847457627119</v>
+      </c>
+      <c r="L50" s="10">
+        <v>1</v>
+      </c>
+      <c r="M50" s="12">
+        <f>IFERROR(IF(J50="",F50,J50)*K50,"")</f>
+        <v>14.1017</v>
+      </c>
+      <c r="N50" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="10" t="s">
         <v>136</v>
       </c>
@@ -2546,7 +3428,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:14">
       <c r="A52" s="10" t="s">
         <v>138</v>
       </c>
@@ -2565,14 +3447,32 @@
       </c>
       <c r="G52" s="11">
         <f>IF(MIN(K52)&lt;&gt;0,MIN(K52),"")</f>
-        <v/>
+        <v>0.05578692493946731</v>
       </c>
       <c r="H52" s="12">
         <f>IF(AND(ISNUMBER(F52),ISNUMBER(G52)),F52*G52,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+        <v>5.5787</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J52" s="10"/>
+      <c r="K52" s="11">
+        <f>IFERROR(IF(OR(J52&gt;=L52,F52&gt;=L52),EUR_USD*LOOKUP(IF(J52="",F52,J52),{0,1,10,100,1000},{0.0,0.164,0.082,0.0576,0.0464}),"MOQ="&amp;L52),"")</f>
+        <v>0.05578692493946731</v>
+      </c>
+      <c r="L52" s="10">
+        <v>1</v>
+      </c>
+      <c r="M52" s="12">
+        <f>IFERROR(IF(J52="",F52,J52)*K52,"")</f>
+        <v>5.5787</v>
+      </c>
+      <c r="N52" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="B54" s="14" t="s">
         <v>150</v>
       </c>
@@ -2595,7 +3495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:14">
       <c r="G55" s="14" t="s">
         <v>149</v>
       </c>
@@ -2604,7 +3504,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:14">
       <c r="A56" s="2" t="s">
         <v>161</v>
       </c>
@@ -2848,647 +3748,732 @@
     <mergeCell ref="J55:M101"/>
   </mergeCells>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="2" priority="15">
+    <cfRule type="expression" dxfId="2" priority="51">
       <formula>AND(ISBLANK(E10),ISBLANK(M10))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="16">
+    <cfRule type="expression" dxfId="1" priority="52">
       <formula>IF(SUM(I10)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
       <formula>SUM(I10)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="54" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K10),J10,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="2" priority="19">
+    <cfRule type="expression" dxfId="2" priority="55">
       <formula>AND(ISBLANK(E11),ISBLANK(M11))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="1" priority="56">
       <formula>IF(SUM(I11)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="greaterThan">
       <formula>SUM(I11)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="58" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K11),J11,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="2" priority="23">
+    <cfRule type="expression" dxfId="2" priority="59">
       <formula>AND(ISBLANK(E12),ISBLANK(M12))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="24">
+    <cfRule type="expression" dxfId="1" priority="60">
       <formula>IF(SUM(I12)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="61" operator="greaterThan">
       <formula>SUM(I12)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="62" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K12),J12,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="2" priority="27">
+    <cfRule type="expression" dxfId="2" priority="63">
       <formula>AND(ISBLANK(E13),ISBLANK(M13))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="28">
+    <cfRule type="expression" dxfId="1" priority="64">
       <formula>IF(SUM(I13)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="greaterThan">
       <formula>SUM(I13)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="66" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K13),J13,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="2" priority="31">
+    <cfRule type="expression" dxfId="2" priority="67">
       <formula>AND(ISBLANK(E14),ISBLANK(M14))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="32">
+    <cfRule type="expression" dxfId="1" priority="68">
       <formula>IF(SUM(I14)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="69" operator="greaterThan">
       <formula>SUM(I14)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="70" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K14),J14,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="2" priority="35">
+    <cfRule type="expression" dxfId="2" priority="71">
       <formula>AND(ISBLANK(E15),ISBLANK(M15))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="36">
+    <cfRule type="expression" dxfId="1" priority="72">
       <formula>IF(SUM(I15)=0,1,0)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="73" operator="greaterThan">
       <formula>SUM(I15)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="74" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K15),J15,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="2" priority="75">
+      <formula>AND(ISBLANK(E16),ISBLANK(M16))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="76">
+      <formula>IF(SUM(I16)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="77" operator="greaterThan">
+      <formula>SUM(I16)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="78" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K16),J16,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="expression" dxfId="2" priority="79">
+      <formula>AND(ISBLANK(E17),ISBLANK(M17))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="80">
+      <formula>IF(SUM(I17)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="81" operator="greaterThan">
+      <formula>SUM(I17)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="82" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K17),J17,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" dxfId="2" priority="83">
+      <formula>AND(ISBLANK(E18),ISBLANK(M18))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="84">
+      <formula>IF(SUM(I18)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="85" operator="greaterThan">
+      <formula>SUM(I18)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="86" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K18),J18,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="expression" dxfId="2" priority="87">
+      <formula>AND(ISBLANK(E19),ISBLANK(M19))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="88">
+      <formula>IF(SUM(I19)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="89" operator="greaterThan">
+      <formula>SUM(I19)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="90" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K19),J19,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="expression" dxfId="2" priority="91">
+      <formula>AND(ISBLANK(E20),ISBLANK(M20))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="92">
+      <formula>IF(SUM(I20)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="93" operator="greaterThan">
+      <formula>SUM(I20)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="94" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K20),J20,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="expression" dxfId="2" priority="95">
+      <formula>AND(ISBLANK(E21),ISBLANK(M21))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="96">
+      <formula>IF(SUM(I21)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="97" operator="greaterThan">
+      <formula>SUM(I21)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="98" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K21),J21,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="expression" dxfId="2" priority="99">
+      <formula>AND(ISBLANK(E22),ISBLANK(M22))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="100">
+      <formula>IF(SUM(I22)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="101" operator="greaterThan">
+      <formula>SUM(I22)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="102" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K22),J22,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="expression" dxfId="2" priority="103">
+      <formula>AND(ISBLANK(E23),ISBLANK(M23))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="104">
+      <formula>IF(SUM(I23)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="105" operator="greaterThan">
+      <formula>SUM(I23)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="106" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K23),J23,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="expression" dxfId="2" priority="107">
+      <formula>AND(ISBLANK(E24),ISBLANK(M24))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="108">
+      <formula>IF(SUM(I24)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="109" operator="greaterThan">
+      <formula>SUM(I24)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="110" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K24),J24,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="expression" dxfId="2" priority="111">
+      <formula>AND(ISBLANK(E25),ISBLANK(M25))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="112">
+      <formula>IF(SUM(I25)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="113" operator="greaterThan">
+      <formula>SUM(I25)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="114" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K25),J25,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="expression" dxfId="2" priority="115">
+      <formula>AND(ISBLANK(E26),ISBLANK(M26))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="116">
+      <formula>IF(SUM(I26)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="117" operator="greaterThan">
+      <formula>SUM(I26)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="118" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K26),J26,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="expression" dxfId="2" priority="119">
+      <formula>AND(ISBLANK(E27),ISBLANK(M27))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="120">
+      <formula>IF(SUM(I27)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="121" operator="greaterThan">
+      <formula>SUM(I27)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="122" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K27),J27,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="expression" dxfId="2" priority="123">
+      <formula>AND(ISBLANK(E28),ISBLANK(M28))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="124">
+      <formula>IF(SUM(I28)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
+      <formula>SUM(I28)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="126" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K28),J28,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="expression" dxfId="2" priority="127">
+      <formula>AND(ISBLANK(E29),ISBLANK(M29))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="128">
+      <formula>IF(SUM(I29)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="129" operator="greaterThan">
+      <formula>SUM(I29)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="130" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K29),J29,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30">
+    <cfRule type="expression" dxfId="2" priority="131">
+      <formula>AND(ISBLANK(E30),ISBLANK(M30))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="132">
+      <formula>IF(SUM(I30)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="133" operator="greaterThan">
+      <formula>SUM(I30)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="134" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K30),J30,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F31">
+    <cfRule type="expression" dxfId="2" priority="135">
+      <formula>AND(ISBLANK(E31),ISBLANK(M31))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="136">
+      <formula>IF(SUM(I31)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="137" operator="greaterThan">
+      <formula>SUM(I31)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="138" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K31),J31,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="expression" dxfId="2" priority="139">
+      <formula>AND(ISBLANK(E32),ISBLANK(M32))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="140">
+      <formula>IF(SUM(I32)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="141" operator="greaterThan">
+      <formula>SUM(I32)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="142" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K32),J32,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F33">
+    <cfRule type="expression" dxfId="2" priority="143">
+      <formula>AND(ISBLANK(E33),ISBLANK(M33))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="144">
+      <formula>IF(SUM(I33)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
+      <formula>SUM(I33)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="146" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K33),J33,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34">
+    <cfRule type="expression" dxfId="2" priority="147">
+      <formula>AND(ISBLANK(E34),ISBLANK(M34))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="148">
+      <formula>IF(SUM(I34)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
+      <formula>SUM(I34)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="150" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K34),J34,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
+    <cfRule type="expression" dxfId="2" priority="151">
+      <formula>AND(ISBLANK(E35),ISBLANK(M35))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="152">
+      <formula>IF(SUM(I35)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
+      <formula>SUM(I35)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="154" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K35),J35,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36">
+    <cfRule type="expression" dxfId="2" priority="155">
+      <formula>AND(ISBLANK(E36),ISBLANK(M36))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="156">
+      <formula>IF(SUM(I36)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="157" operator="greaterThan">
+      <formula>SUM(I36)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="158" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K36),J36,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37">
+    <cfRule type="expression" dxfId="2" priority="159">
+      <formula>AND(ISBLANK(E37),ISBLANK(M37))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="160">
+      <formula>IF(SUM(I37)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="161" operator="greaterThan">
+      <formula>SUM(I37)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="162" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K37),J37,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38">
+    <cfRule type="expression" dxfId="2" priority="163">
+      <formula>AND(ISBLANK(E38),ISBLANK(M38))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="164">
+      <formula>IF(SUM(I38)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="165" operator="greaterThan">
+      <formula>SUM(I38)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="166" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K38),J38,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="expression" dxfId="2" priority="167">
+      <formula>AND(ISBLANK(E39),ISBLANK(M39))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="168">
+      <formula>IF(SUM(I39)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="169" operator="greaterThan">
+      <formula>SUM(I39)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="170" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K39),J39,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
+    <cfRule type="expression" dxfId="2" priority="171">
+      <formula>AND(ISBLANK(E40),ISBLANK(M40))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="172">
+      <formula>IF(SUM(I40)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="173" operator="greaterThan">
+      <formula>SUM(I40)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="174" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K40),J40,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F41">
+    <cfRule type="expression" dxfId="2" priority="175">
+      <formula>AND(ISBLANK(E41),ISBLANK(M41))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="176">
+      <formula>IF(SUM(I41)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="177" operator="greaterThan">
+      <formula>SUM(I41)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="178" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K41),J41,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="expression" dxfId="2" priority="179">
+      <formula>AND(ISBLANK(E42),ISBLANK(M42))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="180">
+      <formula>IF(SUM(I42)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="181" operator="greaterThan">
+      <formula>SUM(I42)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="182" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K42),J42,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F43">
+    <cfRule type="expression" dxfId="2" priority="183">
+      <formula>AND(ISBLANK(E43),ISBLANK(M43))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="184">
+      <formula>IF(SUM(I43)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="185" operator="greaterThan">
+      <formula>SUM(I43)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="186" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K43),J43,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44">
+    <cfRule type="expression" dxfId="2" priority="187">
+      <formula>AND(ISBLANK(E44),ISBLANK(M44))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="188">
+      <formula>IF(SUM(I44)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="189" operator="greaterThan">
+      <formula>SUM(I44)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="190" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K44),J44,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45">
+    <cfRule type="expression" dxfId="2" priority="191">
+      <formula>AND(ISBLANK(E45),ISBLANK(M45))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="192">
+      <formula>IF(SUM(I45)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="193" operator="greaterThan">
+      <formula>SUM(I45)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="194" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K45),J45,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46">
+    <cfRule type="expression" dxfId="2" priority="195">
+      <formula>AND(ISBLANK(E46),ISBLANK(M46))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="196">
+      <formula>IF(SUM(I46)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="197" operator="greaterThan">
+      <formula>SUM(I46)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="198" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K46),J46,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="expression" dxfId="2" priority="199">
+      <formula>AND(ISBLANK(E47),ISBLANK(M47))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="200">
+      <formula>IF(SUM(I47)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="201" operator="greaterThan">
+      <formula>SUM(I47)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="202" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K47),J47,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F48">
+    <cfRule type="expression" dxfId="2" priority="203">
+      <formula>AND(ISBLANK(E48),ISBLANK(M48))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="204">
+      <formula>IF(SUM(I48)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="205" operator="greaterThan">
+      <formula>SUM(I48)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="206" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K48),J48,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F49">
+    <cfRule type="expression" dxfId="2" priority="207">
+      <formula>AND(ISBLANK(E49),ISBLANK(M49))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="208">
+      <formula>IF(SUM(I49)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="209" operator="greaterThan">
+      <formula>SUM(I49)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="210" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K49),J49,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
+    <cfRule type="expression" dxfId="2" priority="211">
+      <formula>AND(ISBLANK(E50),ISBLANK(M50))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="212">
+      <formula>IF(SUM(I50)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="213" operator="greaterThan">
+      <formula>SUM(I50)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="214" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K50),J50,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51">
+    <cfRule type="expression" dxfId="2" priority="215">
+      <formula>AND(ISBLANK(E51),ISBLANK(M51))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="216">
+      <formula>IF(SUM(I51)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="217" operator="greaterThan">
+      <formula>SUM(I51)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="218" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K51),J51,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52">
+    <cfRule type="expression" dxfId="2" priority="219">
+      <formula>AND(ISBLANK(E52),ISBLANK(M52))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="220">
+      <formula>IF(SUM(I52)=0,1,0)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="221" operator="greaterThan">
+      <formula>SUM(I52)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="222" operator="greaterThan">
+      <formula>SUM(IF(ISNUMBER(K52),J52,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
     <cfRule type="expression" dxfId="2" priority="39">
-      <formula>AND(ISBLANK(E16),ISBLANK(M16))</formula>
+      <formula>AND(ISBLANK(E7),ISBLANK(M7))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="40">
-      <formula>IF(SUM(I16)=0,1,0)</formula>
+      <formula>IF(SUM(I7)=0,1,0)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="41" operator="greaterThan">
-      <formula>SUM(I16)</formula>
+      <formula>SUM(I7)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="42" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K16),J16,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
+      <formula>SUM(IF(ISNUMBER(K7),J7,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
     <cfRule type="expression" dxfId="2" priority="43">
-      <formula>AND(ISBLANK(E17),ISBLANK(M17))</formula>
+      <formula>AND(ISBLANK(E8),ISBLANK(M8))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="44">
-      <formula>IF(SUM(I17)=0,1,0)</formula>
+      <formula>IF(SUM(I8)=0,1,0)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="45" operator="greaterThan">
-      <formula>SUM(I17)</formula>
+      <formula>SUM(I8)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="46" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K17),J17,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
+      <formula>SUM(IF(ISNUMBER(K8),J8,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
     <cfRule type="expression" dxfId="2" priority="47">
-      <formula>AND(ISBLANK(E18),ISBLANK(M18))</formula>
+      <formula>AND(ISBLANK(E9),ISBLANK(M9))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="48">
-      <formula>IF(SUM(I18)=0,1,0)</formula>
+      <formula>IF(SUM(I9)=0,1,0)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="49" operator="greaterThan">
-      <formula>SUM(I18)</formula>
+      <formula>SUM(I9)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="50" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K18),J18,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
-    <cfRule type="expression" dxfId="2" priority="51">
-      <formula>AND(ISBLANK(E19),ISBLANK(M19))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="52">
-      <formula>IF(SUM(I19)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="53" operator="greaterThan">
-      <formula>SUM(I19)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="54" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K19),J19,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="expression" dxfId="2" priority="55">
-      <formula>AND(ISBLANK(E20),ISBLANK(M20))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="56">
-      <formula>IF(SUM(I20)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="57" operator="greaterThan">
-      <formula>SUM(I20)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="58" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K20),J20,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="2" priority="59">
-      <formula>AND(ISBLANK(E21),ISBLANK(M21))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="60">
-      <formula>IF(SUM(I21)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="61" operator="greaterThan">
-      <formula>SUM(I21)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="62" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K21),J21,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="2" priority="63">
-      <formula>AND(ISBLANK(E22),ISBLANK(M22))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="64">
-      <formula>IF(SUM(I22)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="65" operator="greaterThan">
-      <formula>SUM(I22)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="66" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K22),J22,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
-    <cfRule type="expression" dxfId="2" priority="67">
-      <formula>AND(ISBLANK(E23),ISBLANK(M23))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="68">
-      <formula>IF(SUM(I23)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="69" operator="greaterThan">
-      <formula>SUM(I23)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="70" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K23),J23,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="expression" dxfId="2" priority="71">
-      <formula>AND(ISBLANK(E24),ISBLANK(M24))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="72">
-      <formula>IF(SUM(I24)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="73" operator="greaterThan">
-      <formula>SUM(I24)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="74" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K24),J24,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25">
-    <cfRule type="expression" dxfId="2" priority="75">
-      <formula>AND(ISBLANK(E25),ISBLANK(M25))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="76">
-      <formula>IF(SUM(I25)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="77" operator="greaterThan">
-      <formula>SUM(I25)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="78" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K25),J25,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="expression" dxfId="2" priority="79">
-      <formula>AND(ISBLANK(E26),ISBLANK(M26))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="80">
-      <formula>IF(SUM(I26)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="81" operator="greaterThan">
-      <formula>SUM(I26)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="82" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K26),J26,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
-    <cfRule type="expression" dxfId="2" priority="83">
-      <formula>AND(ISBLANK(E27),ISBLANK(M27))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="84">
-      <formula>IF(SUM(I27)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="85" operator="greaterThan">
-      <formula>SUM(I27)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="86" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K27),J27,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="2" priority="87">
-      <formula>AND(ISBLANK(E28),ISBLANK(M28))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="88">
-      <formula>IF(SUM(I28)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="89" operator="greaterThan">
-      <formula>SUM(I28)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="90" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K28),J28,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
-    <cfRule type="expression" dxfId="2" priority="91">
-      <formula>AND(ISBLANK(E29),ISBLANK(M29))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="92">
-      <formula>IF(SUM(I29)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="93" operator="greaterThan">
-      <formula>SUM(I29)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="94" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K29),J29,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30">
-    <cfRule type="expression" dxfId="2" priority="95">
-      <formula>AND(ISBLANK(E30),ISBLANK(M30))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="96">
-      <formula>IF(SUM(I30)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="97" operator="greaterThan">
-      <formula>SUM(I30)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="98" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K30),J30,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
-    <cfRule type="expression" dxfId="2" priority="99">
-      <formula>AND(ISBLANK(E31),ISBLANK(M31))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="100">
-      <formula>IF(SUM(I31)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="101" operator="greaterThan">
-      <formula>SUM(I31)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="102" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K31),J31,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
-    <cfRule type="expression" dxfId="2" priority="103">
-      <formula>AND(ISBLANK(E32),ISBLANK(M32))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="104">
-      <formula>IF(SUM(I32)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="105" operator="greaterThan">
-      <formula>SUM(I32)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="106" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K32),J32,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
-    <cfRule type="expression" dxfId="2" priority="107">
-      <formula>AND(ISBLANK(E33),ISBLANK(M33))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="108">
-      <formula>IF(SUM(I33)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="109" operator="greaterThan">
-      <formula>SUM(I33)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="110" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K33),J33,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F34">
-    <cfRule type="expression" dxfId="2" priority="111">
-      <formula>AND(ISBLANK(E34),ISBLANK(M34))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="112">
-      <formula>IF(SUM(I34)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="113" operator="greaterThan">
-      <formula>SUM(I34)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="114" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K34),J34,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
-    <cfRule type="expression" dxfId="2" priority="115">
-      <formula>AND(ISBLANK(E35),ISBLANK(M35))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="116">
-      <formula>IF(SUM(I35)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="117" operator="greaterThan">
-      <formula>SUM(I35)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="118" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K35),J35,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F36">
-    <cfRule type="expression" dxfId="2" priority="119">
-      <formula>AND(ISBLANK(E36),ISBLANK(M36))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="120">
-      <formula>IF(SUM(I36)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="121" operator="greaterThan">
-      <formula>SUM(I36)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="122" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K36),J36,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
-    <cfRule type="expression" dxfId="2" priority="123">
-      <formula>AND(ISBLANK(E37),ISBLANK(M37))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="124">
-      <formula>IF(SUM(I37)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="125" operator="greaterThan">
-      <formula>SUM(I37)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="126" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K37),J37,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
-    <cfRule type="expression" dxfId="2" priority="127">
-      <formula>AND(ISBLANK(E38),ISBLANK(M38))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="128">
-      <formula>IF(SUM(I38)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="129" operator="greaterThan">
-      <formula>SUM(I38)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="130" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K38),J38,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="expression" dxfId="2" priority="131">
-      <formula>AND(ISBLANK(E39),ISBLANK(M39))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="132">
-      <formula>IF(SUM(I39)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="133" operator="greaterThan">
-      <formula>SUM(I39)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="134" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K39),J39,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="expression" dxfId="2" priority="135">
-      <formula>AND(ISBLANK(E40),ISBLANK(M40))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="136">
-      <formula>IF(SUM(I40)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="137" operator="greaterThan">
-      <formula>SUM(I40)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="138" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K40),J40,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
-    <cfRule type="expression" dxfId="2" priority="139">
-      <formula>AND(ISBLANK(E41),ISBLANK(M41))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="140">
-      <formula>IF(SUM(I41)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="141" operator="greaterThan">
-      <formula>SUM(I41)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="142" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K41),J41,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F42">
-    <cfRule type="expression" dxfId="2" priority="143">
-      <formula>AND(ISBLANK(E42),ISBLANK(M42))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="144">
-      <formula>IF(SUM(I42)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="145" operator="greaterThan">
-      <formula>SUM(I42)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="146" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K42),J42,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="2" priority="147">
-      <formula>AND(ISBLANK(E43),ISBLANK(M43))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="148">
-      <formula>IF(SUM(I43)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="149" operator="greaterThan">
-      <formula>SUM(I43)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="150" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K43),J43,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
-    <cfRule type="expression" dxfId="2" priority="151">
-      <formula>AND(ISBLANK(E44),ISBLANK(M44))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="152">
-      <formula>IF(SUM(I44)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="153" operator="greaterThan">
-      <formula>SUM(I44)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="154" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K44),J44,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
-    <cfRule type="expression" dxfId="2" priority="155">
-      <formula>AND(ISBLANK(E45),ISBLANK(M45))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="156">
-      <formula>IF(SUM(I45)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="157" operator="greaterThan">
-      <formula>SUM(I45)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="158" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K45),J45,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F46">
-    <cfRule type="expression" dxfId="2" priority="159">
-      <formula>AND(ISBLANK(E46),ISBLANK(M46))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="160">
-      <formula>IF(SUM(I46)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="161" operator="greaterThan">
-      <formula>SUM(I46)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="162" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K46),J46,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="2" priority="163">
-      <formula>AND(ISBLANK(E47),ISBLANK(M47))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="164">
-      <formula>IF(SUM(I47)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="165" operator="greaterThan">
-      <formula>SUM(I47)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="166" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K47),J47,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="2" priority="167">
-      <formula>AND(ISBLANK(E48),ISBLANK(M48))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="168">
-      <formula>IF(SUM(I48)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="169" operator="greaterThan">
-      <formula>SUM(I48)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="170" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K48),J48,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
-    <cfRule type="expression" dxfId="2" priority="171">
-      <formula>AND(ISBLANK(E49),ISBLANK(M49))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="172">
-      <formula>IF(SUM(I49)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="173" operator="greaterThan">
-      <formula>SUM(I49)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="174" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K49),J49,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="expression" dxfId="2" priority="175">
-      <formula>AND(ISBLANK(E50),ISBLANK(M50))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="176">
-      <formula>IF(SUM(I50)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="177" operator="greaterThan">
-      <formula>SUM(I50)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="178" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K50),J50,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F51">
-    <cfRule type="expression" dxfId="2" priority="179">
-      <formula>AND(ISBLANK(E51),ISBLANK(M51))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="180">
-      <formula>IF(SUM(I51)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="181" operator="greaterThan">
-      <formula>SUM(I51)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="182" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K51),J51,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F52">
-    <cfRule type="expression" dxfId="2" priority="183">
-      <formula>AND(ISBLANK(E52),ISBLANK(M52))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="184">
-      <formula>IF(SUM(I52)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="185" operator="greaterThan">
-      <formula>SUM(I52)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="186" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K52),J52,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>AND(ISBLANK(E7),ISBLANK(M7))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
-      <formula>IF(SUM(I7)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
-      <formula>SUM(I7)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K7),J7,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>AND(ISBLANK(E8),ISBLANK(M8))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>IF(SUM(I8)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
-      <formula>SUM(I8)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="greaterThan">
-      <formula>SUM(IF(ISNUMBER(K8),J8,0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="2" priority="11">
-      <formula>AND(ISBLANK(E9),ISBLANK(M9))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12">
-      <formula>IF(SUM(I9)=0,1,0)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
-      <formula>SUM(I9)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="14" operator="greaterThan">
       <formula>SUM(IF(ISNUMBER(K9),J9,0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThan">
+      <formula>F11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="lessThan">
+      <formula>F12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="lessThan">
+      <formula>F13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="lessThan">
+      <formula>F17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="lessThan">
+      <formula>F19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="lessThan">
+      <formula>F20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I22">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThan">
+      <formula>F22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="lessThan">
+      <formula>F24</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="lessThan">
+      <formula>F25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="lessThan">
+      <formula>F26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="lessThan">
+      <formula>F27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I46">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="lessThan">
+      <formula>F46</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="lessThan">
+      <formula>F47</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I48">
+    <cfRule type="cellIs" dxfId="0" priority="31" operator="lessThan">
+      <formula>F48</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="lessThan">
+      <formula>F49</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I50">
+    <cfRule type="cellIs" dxfId="0" priority="35" operator="lessThan">
+      <formula>F50</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="lessThan">
+      <formula>F52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
@@ -3496,9 +4481,104 @@
       <formula>F7</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I9">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+      <formula>F9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="expression" dxfId="1" priority="6">
+      <formula>AND(NOT(ISBLANK(J11)),OR(I11="NonStk",J11&gt;I11))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J12">
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>AND(NOT(ISBLANK(J12)),OR(I12="NonStk",J12&gt;I12))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="expression" dxfId="1" priority="10">
+      <formula>AND(NOT(ISBLANK(J13)),OR(I13="NonStk",J13&gt;I13))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>AND(NOT(ISBLANK(J17)),OR(I17="NonStk",J17&gt;I17))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="expression" dxfId="1" priority="14">
+      <formula>AND(NOT(ISBLANK(J19)),OR(I19="NonStk",J19&gt;I19))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20">
+    <cfRule type="expression" dxfId="1" priority="16">
+      <formula>AND(NOT(ISBLANK(J20)),OR(I20="NonStk",J20&gt;I20))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J22">
+    <cfRule type="expression" dxfId="1" priority="18">
+      <formula>AND(NOT(ISBLANK(J22)),OR(I22="NonStk",J22&gt;I22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24">
+    <cfRule type="expression" dxfId="1" priority="20">
+      <formula>AND(NOT(ISBLANK(J24)),OR(I24="NonStk",J24&gt;I24))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25">
+    <cfRule type="expression" dxfId="1" priority="22">
+      <formula>AND(NOT(ISBLANK(J25)),OR(I25="NonStk",J25&gt;I25))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26">
+    <cfRule type="expression" dxfId="1" priority="24">
+      <formula>AND(NOT(ISBLANK(J26)),OR(I26="NonStk",J26&gt;I26))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27">
+    <cfRule type="expression" dxfId="1" priority="26">
+      <formula>AND(NOT(ISBLANK(J27)),OR(I27="NonStk",J27&gt;I27))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46">
+    <cfRule type="expression" dxfId="1" priority="28">
+      <formula>AND(NOT(ISBLANK(J46)),OR(I46="NonStk",J46&gt;I46))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47">
+    <cfRule type="expression" dxfId="1" priority="30">
+      <formula>AND(NOT(ISBLANK(J47)),OR(I47="NonStk",J47&gt;I47))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48">
+    <cfRule type="expression" dxfId="1" priority="32">
+      <formula>AND(NOT(ISBLANK(J48)),OR(I48="NonStk",J48&gt;I48))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49">
+    <cfRule type="expression" dxfId="1" priority="34">
+      <formula>AND(NOT(ISBLANK(J49)),OR(I49="NonStk",J49&gt;I49))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J50">
+    <cfRule type="expression" dxfId="1" priority="36">
+      <formula>AND(NOT(ISBLANK(J50)),OR(I50="NonStk",J50&gt;I50))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J52">
+    <cfRule type="expression" dxfId="1" priority="38">
+      <formula>AND(NOT(ISBLANK(J52)),OR(I52="NonStk",J52&gt;I52))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J7">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(NOT(ISBLANK(J7)),OR(I7="NonStk",J7&gt;I7))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>AND(NOT(ISBLANK(J9)),OR(I9="NonStk",J9&gt;I9))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>